<commit_message>
more blade of arcana
</commit_message>
<xml_diff>
--- a/blade-of-arcana/checklist.xlsx
+++ b/blade-of-arcana/checklist.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10810"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10808"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/clark/Local/src/weatherspud/japanese-collectors-list/blade-of-arcana/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E751B6F8-1DDE-954C-886F-C916AAE3E458}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1AB37C7F-A5CE-D940-B97B-C802160E171C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="60" yWindow="460" windowWidth="26740" windowHeight="15780" xr2:uid="{FA770FED-2AE7-3846-B7A2-A9B6EDAC91FE}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="133">
   <si>
     <t>year</t>
   </si>
@@ -330,6 +330,108 @@
   </si>
   <si>
     <t>Super Scenario Supplement Vol. 22</t>
+  </si>
+  <si>
+    <t>ブレイド・オブ・アルカナ The 3rd Edition</t>
+  </si>
+  <si>
+    <t>3rd_edition.jpg</t>
+  </si>
+  <si>
+    <t>Blade of Arcana: The 3rd Edition</t>
+  </si>
+  <si>
+    <t>gate_of_the_brave.jpg</t>
+  </si>
+  <si>
+    <t>ゲート・オブ・ザ・ブレイヴ</t>
+  </si>
+  <si>
+    <t>Gate of the Brave</t>
+  </si>
+  <si>
+    <t>land_of_the_guilty_3rd.jpg</t>
+  </si>
+  <si>
+    <t>sun_of_darkness.jpg</t>
+  </si>
+  <si>
+    <t>サン・オブ・ダークネス</t>
+  </si>
+  <si>
+    <t>Sun of Darkness</t>
+  </si>
+  <si>
+    <t>スレイヤーズ・オブ・レッドドラゴン</t>
+  </si>
+  <si>
+    <t>Slayers of Red Dragon</t>
+  </si>
+  <si>
+    <t>slayers_of_red_dragon.jpg</t>
+  </si>
+  <si>
+    <t>キング・オブ・ザ・ランド</t>
+  </si>
+  <si>
+    <t>King of the Land</t>
+  </si>
+  <si>
+    <t>king_of_the_land.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 剣十字の騎士</t>
+  </si>
+  <si>
+    <t>Knight of the Sword Cross</t>
+  </si>
+  <si>
+    <t>knight_of_the_sword_cross.jpg</t>
+  </si>
+  <si>
+    <t>replay</t>
+  </si>
+  <si>
+    <t>blade_of_arcana_reincarnation.jpg</t>
+  </si>
+  <si>
+    <t>ブレイド・オブ・アルカナ リインカーネイション</t>
+  </si>
+  <si>
+    <t>Blade of Arcana Reincarnation</t>
+  </si>
+  <si>
+    <t>Kadokawa</t>
+  </si>
+  <si>
+    <t>ground_of_valor.jpg</t>
+  </si>
+  <si>
+    <t>グラウンド・オブ・ヴァラー</t>
+  </si>
+  <si>
+    <t>Ground of Valor</t>
+  </si>
+  <si>
+    <t>F.E.A.R.</t>
+  </si>
+  <si>
+    <t>crown_of_evil.jpg</t>
+  </si>
+  <si>
+    <t>クラウン・オブ・イビル</t>
+  </si>
+  <si>
+    <t>Crown of Evil</t>
+  </si>
+  <si>
+    <t>刻まれし者の詩</t>
+  </si>
+  <si>
+    <t>Engraved Poetry</t>
+  </si>
+  <si>
+    <t>engraved_poetry.jpg</t>
   </si>
 </sst>
 </file>
@@ -687,10 +789,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{16AE2C93-B4FB-6A47-9881-D0D1FF4DD6E5}">
-  <dimension ref="A1:F30"/>
+  <dimension ref="A1:F41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9:C30"/>
+      <selection activeCell="A31" sqref="A31:XFD41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -802,42 +904,42 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6">
-        <v>2004</v>
+        <v>2003</v>
       </c>
       <c r="B6" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="C6" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="D6" t="s">
         <v>14</v>
       </c>
       <c r="E6" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="F6" t="s">
-        <v>26</v>
+        <v>15</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7">
-        <v>2003</v>
+        <v>2004</v>
       </c>
       <c r="B7" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="C7" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="D7" t="s">
         <v>14</v>
       </c>
       <c r="E7" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="F7" t="s">
-        <v>15</v>
+        <v>26</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
@@ -993,7 +1095,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B17" t="s">
         <v>63</v>
       </c>
@@ -1010,7 +1112,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B18" t="s">
         <v>64</v>
       </c>
@@ -1027,7 +1129,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="19" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B19" t="s">
         <v>65</v>
       </c>
@@ -1044,7 +1146,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="20" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B20" t="s">
         <v>66</v>
       </c>
@@ -1061,7 +1163,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="21" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B21" t="s">
         <v>67</v>
       </c>
@@ -1078,7 +1180,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="22" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B22" t="s">
         <v>68</v>
       </c>
@@ -1095,7 +1197,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="23" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B23" t="s">
         <v>69</v>
       </c>
@@ -1112,7 +1214,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="24" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B24" t="s">
         <v>70</v>
       </c>
@@ -1129,7 +1231,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="25" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B25" t="s">
         <v>71</v>
       </c>
@@ -1146,7 +1248,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="26" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B26" t="s">
         <v>72</v>
       </c>
@@ -1163,7 +1265,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="27" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B27" t="s">
         <v>73</v>
       </c>
@@ -1180,7 +1282,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="28" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B28" t="s">
         <v>74</v>
       </c>
@@ -1197,7 +1299,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="29" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B29" t="s">
         <v>75</v>
       </c>
@@ -1214,7 +1316,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="30" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B30" t="s">
         <v>76</v>
       </c>
@@ -1231,7 +1333,230 @@
         <v>26</v>
       </c>
     </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A31">
+        <v>2006</v>
+      </c>
+      <c r="B31" t="s">
+        <v>99</v>
+      </c>
+      <c r="C31" t="s">
+        <v>101</v>
+      </c>
+      <c r="D31" t="s">
+        <v>22</v>
+      </c>
+      <c r="E31" t="s">
+        <v>100</v>
+      </c>
+      <c r="F31" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A32">
+        <v>2008</v>
+      </c>
+      <c r="B32" t="s">
+        <v>18</v>
+      </c>
+      <c r="C32" t="s">
+        <v>16</v>
+      </c>
+      <c r="D32" t="s">
+        <v>14</v>
+      </c>
+      <c r="E32" t="s">
+        <v>105</v>
+      </c>
+      <c r="F32" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A33">
+        <v>2008</v>
+      </c>
+      <c r="B33" t="s">
+        <v>107</v>
+      </c>
+      <c r="C33" t="s">
+        <v>108</v>
+      </c>
+      <c r="D33" t="s">
+        <v>14</v>
+      </c>
+      <c r="E33" t="s">
+        <v>106</v>
+      </c>
+      <c r="F33" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A34">
+        <v>2009</v>
+      </c>
+      <c r="B34" t="s">
+        <v>103</v>
+      </c>
+      <c r="C34" t="s">
+        <v>104</v>
+      </c>
+      <c r="D34" t="s">
+        <v>14</v>
+      </c>
+      <c r="E34" t="s">
+        <v>102</v>
+      </c>
+      <c r="F34" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A35">
+        <v>2009</v>
+      </c>
+      <c r="B35" t="s">
+        <v>115</v>
+      </c>
+      <c r="C35" t="s">
+        <v>116</v>
+      </c>
+      <c r="D35" t="s">
+        <v>22</v>
+      </c>
+      <c r="E35" t="s">
+        <v>117</v>
+      </c>
+      <c r="F35" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A36">
+        <v>2010</v>
+      </c>
+      <c r="B36" t="s">
+        <v>109</v>
+      </c>
+      <c r="C36" t="s">
+        <v>110</v>
+      </c>
+      <c r="D36" t="s">
+        <v>22</v>
+      </c>
+      <c r="E36" t="s">
+        <v>111</v>
+      </c>
+      <c r="F36" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A37">
+        <v>2012</v>
+      </c>
+      <c r="B37" t="s">
+        <v>112</v>
+      </c>
+      <c r="C37" t="s">
+        <v>113</v>
+      </c>
+      <c r="D37" t="s">
+        <v>22</v>
+      </c>
+      <c r="E37" t="s">
+        <v>114</v>
+      </c>
+      <c r="F37" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A38">
+        <v>2015</v>
+      </c>
+      <c r="B38" t="s">
+        <v>120</v>
+      </c>
+      <c r="C38" t="s">
+        <v>121</v>
+      </c>
+      <c r="D38" t="s">
+        <v>122</v>
+      </c>
+      <c r="E38" t="s">
+        <v>119</v>
+      </c>
+      <c r="F38" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A39">
+        <v>2015</v>
+      </c>
+      <c r="B39" t="s">
+        <v>124</v>
+      </c>
+      <c r="C39" t="s">
+        <v>125</v>
+      </c>
+      <c r="D39" t="s">
+        <v>126</v>
+      </c>
+      <c r="E39" t="s">
+        <v>123</v>
+      </c>
+      <c r="F39" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A40">
+        <v>2015</v>
+      </c>
+      <c r="B40" t="s">
+        <v>130</v>
+      </c>
+      <c r="C40" t="s">
+        <v>131</v>
+      </c>
+      <c r="D40" t="s">
+        <v>122</v>
+      </c>
+      <c r="E40" t="s">
+        <v>132</v>
+      </c>
+      <c r="F40" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A41">
+        <v>2016</v>
+      </c>
+      <c r="B41" t="s">
+        <v>128</v>
+      </c>
+      <c r="C41" t="s">
+        <v>129</v>
+      </c>
+      <c r="D41" t="s">
+        <v>122</v>
+      </c>
+      <c r="E41" t="s">
+        <v>127</v>
+      </c>
+      <c r="F41" t="s">
+        <v>15</v>
+      </c>
+    </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A31:F41">
+    <sortCondition ref="A31:A41"/>
+  </sortState>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
blade of arcana years
</commit_message>
<xml_diff>
--- a/blade-of-arcana/checklist.xlsx
+++ b/blade-of-arcana/checklist.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10808"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11010"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/clark/Local/src/weatherspud/japanese-collectors-list/blade-of-arcana/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/clark/Local/src/japanese-collectors-list/blade-of-arcana/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1AB37C7F-A5CE-D940-B97B-C802160E171C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1F95DEB-B158-A24D-9DB8-97A202B19687}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="60" yWindow="460" windowWidth="26740" windowHeight="15780" xr2:uid="{FA770FED-2AE7-3846-B7A2-A9B6EDAC91FE}"/>
+    <workbookView xWindow="0" yWindow="600" windowWidth="25480" windowHeight="15780" xr2:uid="{FA770FED-2AE7-3846-B7A2-A9B6EDAC91FE}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -792,7 +792,7 @@
   <dimension ref="A1:F41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A31" sqref="A31:XFD41"/>
+      <selection activeCell="A21" sqref="A21:XFD21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -903,20 +903,17 @@
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A6">
-        <v>2003</v>
-      </c>
       <c r="B6" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="C6" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="D6" t="s">
         <v>14</v>
       </c>
       <c r="E6" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="F6" t="s">
         <v>15</v>
@@ -924,104 +921,119 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7">
-        <v>2004</v>
+        <v>2001</v>
       </c>
       <c r="B7" t="s">
-        <v>23</v>
+        <v>55</v>
       </c>
       <c r="C7" t="s">
-        <v>24</v>
+        <v>77</v>
       </c>
       <c r="D7" t="s">
         <v>14</v>
       </c>
       <c r="E7" t="s">
-        <v>25</v>
+        <v>33</v>
       </c>
       <c r="F7" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>2002</v>
+      </c>
       <c r="B8" t="s">
-        <v>30</v>
+        <v>56</v>
       </c>
       <c r="C8" t="s">
-        <v>31</v>
+        <v>78</v>
       </c>
       <c r="D8" t="s">
         <v>14</v>
       </c>
       <c r="E8" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="F8" t="s">
-        <v>15</v>
+        <v>26</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>2002</v>
+      </c>
       <c r="B9" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="C9" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="D9" t="s">
         <v>14</v>
       </c>
       <c r="E9" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="F9" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>2002</v>
+      </c>
       <c r="B10" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="C10" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="D10" t="s">
         <v>14</v>
       </c>
       <c r="E10" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="F10" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>2002</v>
+      </c>
       <c r="B11" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="C11" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="D11" t="s">
         <v>14</v>
       </c>
       <c r="E11" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="F11" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>2002</v>
+      </c>
       <c r="B12" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="C12" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="D12" t="s">
         <v>14</v>
       </c>
       <c r="E12" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="F12" t="s">
         <v>26</v>
@@ -1029,135 +1041,156 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B13" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="C13" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="D13" t="s">
         <v>14</v>
       </c>
       <c r="E13" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="F13" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>2003</v>
+      </c>
       <c r="B14" t="s">
-        <v>60</v>
+        <v>27</v>
       </c>
       <c r="C14" t="s">
-        <v>82</v>
+        <v>28</v>
       </c>
       <c r="D14" t="s">
         <v>14</v>
       </c>
       <c r="E14" t="s">
-        <v>38</v>
+        <v>29</v>
       </c>
       <c r="F14" t="s">
-        <v>26</v>
+        <v>15</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>2003</v>
+      </c>
       <c r="B15" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C15" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="D15" t="s">
         <v>14</v>
       </c>
       <c r="E15" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="F15" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>2003</v>
+      </c>
       <c r="B16" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C16" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="D16" t="s">
         <v>14</v>
       </c>
       <c r="E16" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="F16" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>2003</v>
+      </c>
       <c r="B17" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="C17" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="D17" t="s">
         <v>14</v>
       </c>
       <c r="E17" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="F17" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A18">
+        <v>2003</v>
+      </c>
       <c r="B18" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="C18" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="D18" t="s">
         <v>14</v>
       </c>
       <c r="E18" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="F18" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A19">
+        <v>2003</v>
+      </c>
       <c r="B19" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C19" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="D19" t="s">
         <v>14</v>
       </c>
       <c r="E19" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="F19" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A20">
+        <v>2003</v>
+      </c>
       <c r="B20" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="C20" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="D20" t="s">
         <v>14</v>
       </c>
       <c r="E20" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="F20" t="s">
         <v>26</v>
@@ -1165,39 +1198,45 @@
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B21" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="C21" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="D21" t="s">
         <v>14</v>
       </c>
       <c r="E21" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="F21" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A22">
+        <v>2004</v>
+      </c>
       <c r="B22" t="s">
-        <v>68</v>
+        <v>23</v>
       </c>
       <c r="C22" t="s">
-        <v>90</v>
+        <v>24</v>
       </c>
       <c r="D22" t="s">
         <v>14</v>
       </c>
       <c r="E22" t="s">
-        <v>46</v>
+        <v>25</v>
       </c>
       <c r="F22" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A23">
+        <v>2004</v>
+      </c>
       <c r="B23" t="s">
         <v>69</v>
       </c>
@@ -1215,6 +1254,9 @@
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A24">
+        <v>2004</v>
+      </c>
       <c r="B24" t="s">
         <v>70</v>
       </c>
@@ -1232,6 +1274,9 @@
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A25">
+        <v>2004</v>
+      </c>
       <c r="B25" t="s">
         <v>71</v>
       </c>
@@ -1249,6 +1294,9 @@
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A26">
+        <v>2004</v>
+      </c>
       <c r="B26" t="s">
         <v>72</v>
       </c>
@@ -1266,6 +1314,9 @@
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A27">
+        <v>2004</v>
+      </c>
       <c r="B27" t="s">
         <v>73</v>
       </c>
@@ -1283,6 +1334,9 @@
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A28">
+        <v>2005</v>
+      </c>
       <c r="B28" t="s">
         <v>74</v>
       </c>
@@ -1300,6 +1354,9 @@
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A29">
+        <v>2005</v>
+      </c>
       <c r="B29" t="s">
         <v>75</v>
       </c>
@@ -1317,6 +1374,9 @@
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A30">
+        <v>2005</v>
+      </c>
       <c r="B30" t="s">
         <v>76</v>
       </c>
@@ -1554,8 +1614,8 @@
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A31:F41">
-    <sortCondition ref="A31:A41"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F44">
+    <sortCondition ref="A2:A44"/>
   </sortState>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>